<commit_message>
Add marketing tag to temlate
</commit_message>
<xml_diff>
--- a/wine2.xlsx
+++ b/wine2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a18387289/Documents/DEV/wine_project/wine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459BA517-0F76-1547-B1E6-2D9B5F7297EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE45312-323A-8F49-B49D-61637F7DAAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13480" yWindow="2520" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12580" yWindow="2520" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Название</t>
   </si>
@@ -426,10 +426,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A14" sqref="A14:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -656,6 +656,57 @@
         <v>39</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3">
+        <v>200</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3">
+        <v>150</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3">
+        <v>150</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>